<commit_message>
the phrases screen now shows the category in the title.
</commit_message>
<xml_diff>
--- a/app/src/main/assets/Cantonese Phrases.xlsx
+++ b/app/src/main/assets/Cantonese Phrases.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2449" uniqueCount="1643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2449" uniqueCount="1644">
   <si>
     <t>Basics</t>
   </si>
@@ -4530,9 +4530,6 @@
     <t>我想換過間房</t>
   </si>
   <si>
-    <t>ngóh séung wuhngwo gàanfóng</t>
-  </si>
-  <si>
     <t>When should I vacate the room?</t>
   </si>
   <si>
@@ -4716,18 +4713,12 @@
     <t>你好靚。</t>
   </si>
   <si>
-    <t xml:space="preserve"> I think of you as more than a friend. </t>
-  </si>
-  <si>
     <t>我當你係朋友咋。</t>
   </si>
   <si>
     <t xml:space="preserve">A hundred hearts would be too few to carry all my love for you. </t>
   </si>
   <si>
-    <t>一百個心都裝唔晒我對你嘅</t>
-  </si>
-  <si>
     <t>You're so handsome.</t>
   </si>
   <si>
@@ -4740,9 +4731,6 @@
     <t>我暗戀你。</t>
   </si>
   <si>
-    <t xml:space="preserve"> You make me want to be a better man. </t>
-  </si>
-  <si>
     <t>你令我想成為一個更好嘅</t>
   </si>
   <si>
@@ -4827,9 +4815,6 @@
     <t>Headache</t>
   </si>
   <si>
-    <t>tau4 tung3</t>
-  </si>
-  <si>
     <t>頭痛</t>
   </si>
   <si>
@@ -4839,27 +4824,18 @@
     <t>肚痛</t>
   </si>
   <si>
-    <t>tou5 tung3</t>
-  </si>
-  <si>
     <t>藥</t>
   </si>
   <si>
     <t>Medicine</t>
   </si>
   <si>
-    <t>joek6</t>
-  </si>
-  <si>
     <t>Pharmacy</t>
   </si>
   <si>
     <t>藥房</t>
   </si>
   <si>
-    <t>joek6 fong4</t>
-  </si>
-  <si>
     <t>Doctor</t>
   </si>
   <si>
@@ -4872,18 +4848,12 @@
     <t>白車</t>
   </si>
   <si>
-    <t>baak6 ce1</t>
-  </si>
-  <si>
     <t>醫院</t>
   </si>
   <si>
     <t>Hospital</t>
   </si>
   <si>
-    <t>ji1 jyun6*2</t>
-  </si>
-  <si>
     <t>Help me</t>
   </si>
   <si>
@@ -4908,45 +4878,30 @@
     <t>意外</t>
   </si>
   <si>
-    <t>ji3 ngoi6</t>
-  </si>
-  <si>
     <t>爆血管</t>
   </si>
   <si>
     <t>Stroke</t>
   </si>
   <si>
-    <t>baau3 hyut3 gun2</t>
-  </si>
-  <si>
     <t>Heart Attack</t>
   </si>
   <si>
     <t>心臟病發</t>
   </si>
   <si>
-    <t>sam1 zong6 beng6 faat</t>
-  </si>
-  <si>
     <t>Asthma</t>
   </si>
   <si>
     <t>氣喘病</t>
   </si>
   <si>
-    <t>hei3 cyun2 beng6</t>
-  </si>
-  <si>
     <t>Allergy</t>
   </si>
   <si>
     <t>過敏</t>
   </si>
   <si>
-    <t>gwo3 man5</t>
-  </si>
-  <si>
     <t>file:///android_asset/medical.png</t>
   </si>
   <si>
@@ -4954,6 +4909,54 @@
   </si>
   <si>
     <t>fo gei m̀h' gōi.</t>
+  </si>
+  <si>
+    <t>ngóh séung wuhn gwo gàan fóng</t>
+  </si>
+  <si>
+    <t>一百個心都裝唔晒我對你嘅愛</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I think of you as more than a friend. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">You make me want to be a better man. </t>
+  </si>
+  <si>
+    <t>baau hyut gun</t>
+  </si>
+  <si>
+    <t>tau tung</t>
+  </si>
+  <si>
+    <t>tou tung</t>
+  </si>
+  <si>
+    <t>gwo man</t>
+  </si>
+  <si>
+    <t>joek</t>
+  </si>
+  <si>
+    <t>joek fong</t>
+  </si>
+  <si>
+    <t>baak ce</t>
+  </si>
+  <si>
+    <t>ji jyun*</t>
+  </si>
+  <si>
+    <t>ji ngoi</t>
+  </si>
+  <si>
+    <t>sam zong beng faat</t>
+  </si>
+  <si>
+    <t>hei cyun beng</t>
+  </si>
+  <si>
+    <t>file:///android_asset/driving.png</t>
   </si>
 </sst>
 </file>
@@ -5296,8 +5299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F413"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A385" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E312" sqref="E312"/>
+    <sheetView tabSelected="1" topLeftCell="A366" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A370" sqref="A370"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5506,13 +5509,13 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
+        <v>1538</v>
+      </c>
+      <c r="D10" t="s">
         <v>1539</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>1540</v>
-      </c>
-      <c r="E10" t="s">
-        <v>1541</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>427</v>
@@ -5527,13 +5530,13 @@
         <v>0</v>
       </c>
       <c r="C11" t="s">
+        <v>1541</v>
+      </c>
+      <c r="D11" t="s">
         <v>1542</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>1543</v>
-      </c>
-      <c r="E11" t="s">
-        <v>1544</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>427</v>
@@ -5548,13 +5551,13 @@
         <v>0</v>
       </c>
       <c r="C12" t="s">
+        <v>1544</v>
+      </c>
+      <c r="D12" t="s">
         <v>1545</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>1546</v>
-      </c>
-      <c r="E12" t="s">
-        <v>1547</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>427</v>
@@ -5569,13 +5572,13 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
+        <v>1547</v>
+      </c>
+      <c r="D13" t="s">
         <v>1548</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>1549</v>
-      </c>
-      <c r="E13" t="s">
-        <v>1550</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>427</v>
@@ -6037,7 +6040,7 @@
         <v>1465</v>
       </c>
       <c r="E35" t="s">
-        <v>1592</v>
+        <v>1588</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>427</v>
@@ -6094,13 +6097,13 @@
         <v>0</v>
       </c>
       <c r="C38" t="s">
+        <v>1550</v>
+      </c>
+      <c r="D38" t="s">
         <v>1551</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>1552</v>
-      </c>
-      <c r="E38" t="s">
-        <v>1553</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>427</v>
@@ -6154,7 +6157,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>1595</v>
+        <v>1591</v>
       </c>
       <c r="C41" t="s">
         <v>467</v>
@@ -6175,7 +6178,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>1595</v>
+        <v>1591</v>
       </c>
       <c r="C42" t="s">
         <v>468</v>
@@ -6196,7 +6199,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>1595</v>
+        <v>1591</v>
       </c>
       <c r="C43" t="s">
         <v>469</v>
@@ -6217,7 +6220,7 @@
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>1595</v>
+        <v>1591</v>
       </c>
       <c r="C44" t="s">
         <v>470</v>
@@ -6238,7 +6241,7 @@
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>1595</v>
+        <v>1591</v>
       </c>
       <c r="C45" t="s">
         <v>1475</v>
@@ -6259,7 +6262,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>1595</v>
+        <v>1591</v>
       </c>
       <c r="C46" t="s">
         <v>471</v>
@@ -6280,7 +6283,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>1595</v>
+        <v>1591</v>
       </c>
       <c r="C47" t="s">
         <v>1472</v>
@@ -6301,7 +6304,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>1595</v>
+        <v>1591</v>
       </c>
       <c r="C48" t="s">
         <v>472</v>
@@ -6322,7 +6325,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>1595</v>
+        <v>1591</v>
       </c>
       <c r="C49" t="s">
         <v>473</v>
@@ -6343,7 +6346,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>1595</v>
+        <v>1591</v>
       </c>
       <c r="C50" t="s">
         <v>474</v>
@@ -6364,7 +6367,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>1595</v>
+        <v>1591</v>
       </c>
       <c r="C51" t="s">
         <v>475</v>
@@ -6385,7 +6388,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>1595</v>
+        <v>1591</v>
       </c>
       <c r="C52" t="s">
         <v>476</v>
@@ -6406,7 +6409,7 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>1598</v>
+        <v>1594</v>
       </c>
       <c r="C53" t="s">
         <v>477</v>
@@ -6427,7 +6430,7 @@
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>1598</v>
+        <v>1594</v>
       </c>
       <c r="C54" t="s">
         <v>478</v>
@@ -6448,7 +6451,7 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>1598</v>
+        <v>1594</v>
       </c>
       <c r="C55" t="s">
         <v>479</v>
@@ -6469,7 +6472,7 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>1595</v>
+        <v>1591</v>
       </c>
       <c r="C56" t="s">
         <v>480</v>
@@ -6490,7 +6493,7 @@
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>1595</v>
+        <v>1591</v>
       </c>
       <c r="C57" t="s">
         <v>481</v>
@@ -6511,7 +6514,7 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>1595</v>
+        <v>1591</v>
       </c>
       <c r="C58" t="s">
         <v>482</v>
@@ -6532,7 +6535,7 @@
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>1595</v>
+        <v>1591</v>
       </c>
       <c r="C59" t="s">
         <v>483</v>
@@ -6553,7 +6556,7 @@
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>1595</v>
+        <v>1591</v>
       </c>
       <c r="C60" t="s">
         <v>484</v>
@@ -6574,7 +6577,7 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>1595</v>
+        <v>1591</v>
       </c>
       <c r="C61" t="s">
         <v>485</v>
@@ -6595,7 +6598,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>1595</v>
+        <v>1591</v>
       </c>
       <c r="C62" t="s">
         <v>486</v>
@@ -6616,7 +6619,7 @@
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>1595</v>
+        <v>1591</v>
       </c>
       <c r="C63" t="s">
         <v>487</v>
@@ -6637,7 +6640,7 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>1595</v>
+        <v>1591</v>
       </c>
       <c r="C64" t="s">
         <v>488</v>
@@ -8032,7 +8035,7 @@
         <v>1215</v>
       </c>
       <c r="E130" t="s">
-        <v>1588</v>
+        <v>1584</v>
       </c>
       <c r="F130" s="1" t="s">
         <v>430</v>
@@ -8074,7 +8077,7 @@
         <v>1217</v>
       </c>
       <c r="E132" t="s">
-        <v>1589</v>
+        <v>1585</v>
       </c>
       <c r="F132" s="1" t="s">
         <v>430</v>
@@ -8095,7 +8098,7 @@
         <v>1218</v>
       </c>
       <c r="E133" t="s">
-        <v>1590</v>
+        <v>1586</v>
       </c>
       <c r="F133" s="1" t="s">
         <v>430</v>
@@ -9061,7 +9064,7 @@
         <v>1264</v>
       </c>
       <c r="E179" t="s">
-        <v>1591</v>
+        <v>1587</v>
       </c>
       <c r="F179" s="1" t="s">
         <v>432</v>
@@ -9964,7 +9967,7 @@
         <v>1500</v>
       </c>
       <c r="E222" t="s">
-        <v>1501</v>
+        <v>1628</v>
       </c>
       <c r="F222" s="1" t="s">
         <v>433</v>
@@ -9979,13 +9982,13 @@
         <v>397</v>
       </c>
       <c r="C223" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D223" t="s">
         <v>1502</v>
       </c>
-      <c r="D223" t="s">
+      <c r="E223" t="s">
         <v>1503</v>
-      </c>
-      <c r="E223" t="s">
-        <v>1504</v>
       </c>
       <c r="F223" s="1" t="s">
         <v>433</v>
@@ -10627,7 +10630,7 @@
         <v>254</v>
       </c>
       <c r="B254" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C254" t="s">
         <v>399</v>
@@ -10648,7 +10651,7 @@
         <v>255</v>
       </c>
       <c r="B255" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C255" t="s">
         <v>400</v>
@@ -10669,7 +10672,7 @@
         <v>256</v>
       </c>
       <c r="B256" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C256" t="s">
         <v>401</v>
@@ -10690,7 +10693,7 @@
         <v>257</v>
       </c>
       <c r="B257" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C257" t="s">
         <v>402</v>
@@ -10711,7 +10714,7 @@
         <v>258</v>
       </c>
       <c r="B258" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C258" t="s">
         <v>403</v>
@@ -10732,7 +10735,7 @@
         <v>259</v>
       </c>
       <c r="B259" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C259" t="s">
         <v>404</v>
@@ -10753,7 +10756,7 @@
         <v>260</v>
       </c>
       <c r="B260" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C260" t="s">
         <v>405</v>
@@ -10774,7 +10777,7 @@
         <v>261</v>
       </c>
       <c r="B261" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C261" t="s">
         <v>406</v>
@@ -10906,10 +10909,10 @@
         <v>676</v>
       </c>
       <c r="D267" t="s">
+        <v>1510</v>
+      </c>
+      <c r="E267" t="s">
         <v>1511</v>
-      </c>
-      <c r="E267" t="s">
-        <v>1512</v>
       </c>
       <c r="F267" s="1" t="s">
         <v>435</v>
@@ -11029,13 +11032,13 @@
         <v>423</v>
       </c>
       <c r="C273" t="s">
+        <v>1504</v>
+      </c>
+      <c r="D273" t="s">
         <v>1505</v>
       </c>
-      <c r="D273" t="s">
+      <c r="E273" t="s">
         <v>1506</v>
-      </c>
-      <c r="E273" t="s">
-        <v>1507</v>
       </c>
       <c r="F273" s="1" t="s">
         <v>435</v>
@@ -11050,13 +11053,13 @@
         <v>423</v>
       </c>
       <c r="C274" t="s">
+        <v>1507</v>
+      </c>
+      <c r="D274" t="s">
         <v>1508</v>
       </c>
-      <c r="D274" t="s">
+      <c r="E274" t="s">
         <v>1509</v>
-      </c>
-      <c r="E274" t="s">
-        <v>1510</v>
       </c>
       <c r="F274" s="1" t="s">
         <v>435</v>
@@ -11194,7 +11197,7 @@
         <v>281</v>
       </c>
       <c r="B281" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C281" t="s">
         <v>687</v>
@@ -11215,7 +11218,7 @@
         <v>282</v>
       </c>
       <c r="B282" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C282" t="s">
         <v>688</v>
@@ -11236,7 +11239,7 @@
         <v>283</v>
       </c>
       <c r="B283" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C283" t="s">
         <v>689</v>
@@ -11257,7 +11260,7 @@
         <v>284</v>
       </c>
       <c r="B284" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C284" t="s">
         <v>690</v>
@@ -11278,7 +11281,7 @@
         <v>285</v>
       </c>
       <c r="B285" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C285" t="s">
         <v>691</v>
@@ -11299,7 +11302,7 @@
         <v>286</v>
       </c>
       <c r="B286" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C286" t="s">
         <v>692</v>
@@ -11320,7 +11323,7 @@
         <v>287</v>
       </c>
       <c r="B287" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C287" t="s">
         <v>693</v>
@@ -11341,7 +11344,7 @@
         <v>288</v>
       </c>
       <c r="B288" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C288" t="s">
         <v>694</v>
@@ -11362,7 +11365,7 @@
         <v>289</v>
       </c>
       <c r="B289" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C289" t="s">
         <v>695</v>
@@ -11383,7 +11386,7 @@
         <v>290</v>
       </c>
       <c r="B290" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C290" t="s">
         <v>696</v>
@@ -11404,7 +11407,7 @@
         <v>291</v>
       </c>
       <c r="B291" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C291" t="s">
         <v>697</v>
@@ -11425,7 +11428,7 @@
         <v>292</v>
       </c>
       <c r="B292" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C292" t="s">
         <v>698</v>
@@ -11446,7 +11449,7 @@
         <v>293</v>
       </c>
       <c r="B293" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C293" t="s">
         <v>699</v>
@@ -11467,7 +11470,7 @@
         <v>294</v>
       </c>
       <c r="B294" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C294" t="s">
         <v>700</v>
@@ -11488,7 +11491,7 @@
         <v>295</v>
       </c>
       <c r="B295" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C295" t="s">
         <v>701</v>
@@ -11509,7 +11512,7 @@
         <v>296</v>
       </c>
       <c r="B296" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C296" t="s">
         <v>702</v>
@@ -11530,7 +11533,7 @@
         <v>297</v>
       </c>
       <c r="B297" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C297" t="s">
         <v>703</v>
@@ -11551,7 +11554,7 @@
         <v>298</v>
       </c>
       <c r="B298" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C298" t="s">
         <v>704</v>
@@ -11572,7 +11575,7 @@
         <v>299</v>
       </c>
       <c r="B299" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C299" t="s">
         <v>705</v>
@@ -11593,7 +11596,7 @@
         <v>300</v>
       </c>
       <c r="B300" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C300" t="s">
         <v>706</v>
@@ -11614,7 +11617,7 @@
         <v>301</v>
       </c>
       <c r="B301" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C301" t="s">
         <v>707</v>
@@ -11635,7 +11638,7 @@
         <v>302</v>
       </c>
       <c r="B302" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C302" t="s">
         <v>708</v>
@@ -11656,7 +11659,7 @@
         <v>303</v>
       </c>
       <c r="B303" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C303" t="s">
         <v>709</v>
@@ -11677,7 +11680,7 @@
         <v>304</v>
       </c>
       <c r="B304" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C304" t="s">
         <v>710</v>
@@ -11698,7 +11701,7 @@
         <v>305</v>
       </c>
       <c r="B305" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C305" t="s">
         <v>711</v>
@@ -11719,7 +11722,7 @@
         <v>306</v>
       </c>
       <c r="B306" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C306" t="s">
         <v>712</v>
@@ -11740,7 +11743,7 @@
         <v>307</v>
       </c>
       <c r="B307" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C307" t="s">
         <v>713</v>
@@ -11761,7 +11764,7 @@
         <v>308</v>
       </c>
       <c r="B308" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C308" t="s">
         <v>714</v>
@@ -11782,7 +11785,7 @@
         <v>309</v>
       </c>
       <c r="B309" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C309" t="s">
         <v>715</v>
@@ -11803,7 +11806,7 @@
         <v>310</v>
       </c>
       <c r="B310" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C310" t="s">
         <v>716</v>
@@ -11830,10 +11833,10 @@
         <v>717</v>
       </c>
       <c r="D311" t="s">
-        <v>1641</v>
+        <v>1626</v>
       </c>
       <c r="E311" t="s">
-        <v>1642</v>
+        <v>1627</v>
       </c>
       <c r="F311" s="1" t="s">
         <v>435</v>
@@ -13045,13 +13048,13 @@
         <v>425</v>
       </c>
       <c r="C369" t="s">
+        <v>1553</v>
+      </c>
+      <c r="D369" t="s">
         <v>1554</v>
       </c>
-      <c r="D369" t="s">
+      <c r="E369" t="s">
         <v>1555</v>
-      </c>
-      <c r="E369" t="s">
-        <v>1556</v>
       </c>
       <c r="F369" s="1" t="s">
         <v>437</v>
@@ -13063,7 +13066,7 @@
         <v>370</v>
       </c>
       <c r="B370" t="s">
-        <v>1597</v>
+        <v>1593</v>
       </c>
       <c r="C370" t="s">
         <v>773</v>
@@ -13075,7 +13078,7 @@
         <v>1095</v>
       </c>
       <c r="F370" s="1" t="s">
-        <v>432</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="371" spans="1:6" x14ac:dyDescent="0.3">
@@ -13084,7 +13087,7 @@
         <v>371</v>
       </c>
       <c r="B371" t="s">
-        <v>1597</v>
+        <v>1593</v>
       </c>
       <c r="C371" t="s">
         <v>774</v>
@@ -13096,7 +13099,7 @@
         <v>1096</v>
       </c>
       <c r="F371" s="1" t="s">
-        <v>432</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="372" spans="1:6" x14ac:dyDescent="0.3">
@@ -13105,7 +13108,7 @@
         <v>372</v>
       </c>
       <c r="B372" t="s">
-        <v>1597</v>
+        <v>1593</v>
       </c>
       <c r="C372" t="s">
         <v>775</v>
@@ -13117,7 +13120,7 @@
         <v>1097</v>
       </c>
       <c r="F372" s="1" t="s">
-        <v>432</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="373" spans="1:6" x14ac:dyDescent="0.3">
@@ -13126,7 +13129,7 @@
         <v>373</v>
       </c>
       <c r="B373" t="s">
-        <v>1597</v>
+        <v>1593</v>
       </c>
       <c r="C373" t="s">
         <v>776</v>
@@ -13138,7 +13141,7 @@
         <v>1098</v>
       </c>
       <c r="F373" s="1" t="s">
-        <v>432</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="374" spans="1:6" x14ac:dyDescent="0.3">
@@ -13147,7 +13150,7 @@
         <v>374</v>
       </c>
       <c r="B374" t="s">
-        <v>1597</v>
+        <v>1593</v>
       </c>
       <c r="C374" t="s">
         <v>777</v>
@@ -13159,7 +13162,7 @@
         <v>1099</v>
       </c>
       <c r="F374" s="1" t="s">
-        <v>432</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="375" spans="1:6" x14ac:dyDescent="0.3">
@@ -13168,7 +13171,7 @@
         <v>375</v>
       </c>
       <c r="B375" t="s">
-        <v>1597</v>
+        <v>1593</v>
       </c>
       <c r="C375" t="s">
         <v>778</v>
@@ -13180,7 +13183,7 @@
         <v>1100</v>
       </c>
       <c r="F375" s="1" t="s">
-        <v>432</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="376" spans="1:6" x14ac:dyDescent="0.3">
@@ -13189,7 +13192,7 @@
         <v>376</v>
       </c>
       <c r="B376" t="s">
-        <v>1597</v>
+        <v>1593</v>
       </c>
       <c r="C376" t="s">
         <v>779</v>
@@ -13201,7 +13204,7 @@
         <v>1101</v>
       </c>
       <c r="F376" s="1" t="s">
-        <v>432</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="377" spans="1:6" x14ac:dyDescent="0.3">
@@ -13210,7 +13213,7 @@
         <v>377</v>
       </c>
       <c r="B377" t="s">
-        <v>1597</v>
+        <v>1593</v>
       </c>
       <c r="C377" t="s">
         <v>780</v>
@@ -13222,7 +13225,7 @@
         <v>1102</v>
       </c>
       <c r="F377" s="1" t="s">
-        <v>432</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="378" spans="1:6" x14ac:dyDescent="0.3">
@@ -13231,7 +13234,7 @@
         <v>378</v>
       </c>
       <c r="B378" t="s">
-        <v>1597</v>
+        <v>1593</v>
       </c>
       <c r="C378" t="s">
         <v>781</v>
@@ -13243,7 +13246,7 @@
         <v>1103</v>
       </c>
       <c r="F378" s="1" t="s">
-        <v>432</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="379" spans="1:6" x14ac:dyDescent="0.3">
@@ -13252,7 +13255,7 @@
         <v>379</v>
       </c>
       <c r="B379" t="s">
-        <v>1597</v>
+        <v>1593</v>
       </c>
       <c r="C379" t="s">
         <v>782</v>
@@ -13264,7 +13267,7 @@
         <v>1104</v>
       </c>
       <c r="F379" s="1" t="s">
-        <v>432</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="380" spans="1:6" x14ac:dyDescent="0.3">
@@ -13273,7 +13276,7 @@
         <v>380</v>
       </c>
       <c r="B380" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="C380" t="s">
         <v>1469</v>
@@ -13285,7 +13288,7 @@
         <v>1471</v>
       </c>
       <c r="F380" s="1" t="s">
-        <v>1577</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="381" spans="1:6" x14ac:dyDescent="0.3">
@@ -13294,19 +13297,19 @@
         <v>381</v>
       </c>
       <c r="B381" t="s">
+        <v>1512</v>
+      </c>
+      <c r="C381" t="s">
         <v>1513</v>
       </c>
-      <c r="C381" t="s">
+      <c r="D381" t="s">
         <v>1514</v>
       </c>
-      <c r="D381" t="s">
+      <c r="E381" t="s">
         <v>1515</v>
       </c>
-      <c r="E381" t="s">
-        <v>1516</v>
-      </c>
       <c r="F381" s="1" t="s">
-        <v>1577</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="382" spans="1:6" x14ac:dyDescent="0.3">
@@ -13315,19 +13318,19 @@
         <v>382</v>
       </c>
       <c r="B382" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="C382" t="s">
+        <v>1516</v>
+      </c>
+      <c r="D382" t="s">
         <v>1517</v>
       </c>
-      <c r="D382" t="s">
-        <v>1518</v>
-      </c>
       <c r="E382" t="s">
-        <v>1593</v>
+        <v>1589</v>
       </c>
       <c r="F382" s="1" t="s">
-        <v>1577</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="383" spans="1:6" x14ac:dyDescent="0.3">
@@ -13336,19 +13339,19 @@
         <v>383</v>
       </c>
       <c r="B383" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="C383" t="s">
+        <v>1518</v>
+      </c>
+      <c r="D383" t="s">
         <v>1519</v>
       </c>
-      <c r="D383" t="s">
+      <c r="E383" t="s">
         <v>1520</v>
       </c>
-      <c r="E383" t="s">
-        <v>1521</v>
-      </c>
       <c r="F383" s="1" t="s">
-        <v>1577</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="384" spans="1:6" x14ac:dyDescent="0.3">
@@ -13357,19 +13360,19 @@
         <v>384</v>
       </c>
       <c r="B384" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="C384" t="s">
+        <v>1521</v>
+      </c>
+      <c r="D384" t="s">
         <v>1522</v>
       </c>
-      <c r="D384" t="s">
+      <c r="E384" t="s">
         <v>1523</v>
       </c>
-      <c r="E384" t="s">
-        <v>1524</v>
-      </c>
       <c r="F384" s="1" t="s">
-        <v>1577</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="385" spans="1:6" x14ac:dyDescent="0.3">
@@ -13378,19 +13381,19 @@
         <v>385</v>
       </c>
       <c r="B385" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="C385" t="s">
+        <v>1524</v>
+      </c>
+      <c r="D385" t="s">
         <v>1525</v>
       </c>
-      <c r="D385" t="s">
+      <c r="E385" t="s">
         <v>1526</v>
       </c>
-      <c r="E385" t="s">
-        <v>1527</v>
-      </c>
       <c r="F385" s="1" t="s">
-        <v>1577</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="386" spans="1:6" x14ac:dyDescent="0.3">
@@ -13399,19 +13402,19 @@
         <v>386</v>
       </c>
       <c r="B386" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="C386" t="s">
+        <v>1527</v>
+      </c>
+      <c r="D386" t="s">
         <v>1528</v>
       </c>
-      <c r="D386" t="s">
-        <v>1529</v>
-      </c>
       <c r="E386" t="s">
-        <v>1594</v>
+        <v>1590</v>
       </c>
       <c r="F386" s="1" t="s">
-        <v>1577</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="387" spans="1:6" x14ac:dyDescent="0.3">
@@ -13420,19 +13423,19 @@
         <v>387</v>
       </c>
       <c r="B387" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="C387" t="s">
+        <v>1529</v>
+      </c>
+      <c r="D387" t="s">
         <v>1530</v>
       </c>
-      <c r="D387" t="s">
+      <c r="E387" t="s">
         <v>1531</v>
       </c>
-      <c r="E387" t="s">
-        <v>1532</v>
-      </c>
       <c r="F387" s="1" t="s">
-        <v>1577</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="388" spans="1:6" x14ac:dyDescent="0.3">
@@ -13441,19 +13444,19 @@
         <v>388</v>
       </c>
       <c r="B388" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="C388" t="s">
+        <v>1532</v>
+      </c>
+      <c r="D388" t="s">
         <v>1533</v>
       </c>
-      <c r="D388" t="s">
+      <c r="E388" t="s">
         <v>1534</v>
       </c>
-      <c r="E388" t="s">
-        <v>1535</v>
-      </c>
       <c r="F388" s="1" t="s">
-        <v>1577</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="389" spans="1:6" x14ac:dyDescent="0.3">
@@ -13462,19 +13465,19 @@
         <v>389</v>
       </c>
       <c r="B389" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="C389" t="s">
+        <v>1535</v>
+      </c>
+      <c r="D389" t="s">
         <v>1536</v>
       </c>
-      <c r="D389" t="s">
+      <c r="E389" t="s">
         <v>1537</v>
       </c>
-      <c r="E389" t="s">
-        <v>1538</v>
-      </c>
       <c r="F389" s="1" t="s">
-        <v>1577</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="390" spans="1:6" x14ac:dyDescent="0.3">
@@ -13483,19 +13486,19 @@
         <v>390</v>
       </c>
       <c r="B390" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="C390" t="s">
+        <v>1556</v>
+      </c>
+      <c r="D390" t="s">
         <v>1557</v>
       </c>
-      <c r="D390" t="s">
-        <v>1558</v>
-      </c>
       <c r="E390" t="s">
-        <v>1582</v>
+        <v>1578</v>
       </c>
       <c r="F390" s="1" t="s">
-        <v>1577</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="391" spans="1:6" x14ac:dyDescent="0.3">
@@ -13504,19 +13507,19 @@
         <v>391</v>
       </c>
       <c r="B391" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="C391" t="s">
+        <v>1558</v>
+      </c>
+      <c r="D391" t="s">
         <v>1559</v>
       </c>
-      <c r="D391" t="s">
-        <v>1560</v>
-      </c>
       <c r="E391" t="s">
-        <v>1583</v>
+        <v>1579</v>
       </c>
       <c r="F391" s="1" t="s">
-        <v>1577</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="392" spans="1:6" x14ac:dyDescent="0.3">
@@ -13525,19 +13528,19 @@
         <v>392</v>
       </c>
       <c r="B392" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="C392" t="s">
+        <v>1560</v>
+      </c>
+      <c r="D392" t="s">
         <v>1561</v>
       </c>
-      <c r="D392" t="s">
-        <v>1562</v>
-      </c>
       <c r="E392" t="s">
-        <v>1578</v>
+        <v>1574</v>
       </c>
       <c r="F392" s="1" t="s">
-        <v>1577</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="393" spans="1:6" x14ac:dyDescent="0.3">
@@ -13546,19 +13549,19 @@
         <v>393</v>
       </c>
       <c r="B393" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="C393" t="s">
-        <v>1563</v>
+        <v>1630</v>
       </c>
       <c r="D393" t="s">
-        <v>1564</v>
+        <v>1562</v>
       </c>
       <c r="E393" t="s">
-        <v>1584</v>
+        <v>1580</v>
       </c>
       <c r="F393" s="1" t="s">
-        <v>1577</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="394" spans="1:6" x14ac:dyDescent="0.3">
@@ -13567,19 +13570,19 @@
         <v>394</v>
       </c>
       <c r="B394" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="C394" t="s">
-        <v>1565</v>
+        <v>1563</v>
       </c>
       <c r="D394" t="s">
-        <v>1566</v>
+        <v>1629</v>
       </c>
       <c r="E394" t="s">
-        <v>1579</v>
+        <v>1575</v>
       </c>
       <c r="F394" s="1" t="s">
-        <v>1577</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="395" spans="1:6" x14ac:dyDescent="0.3">
@@ -13588,19 +13591,19 @@
         <v>395</v>
       </c>
       <c r="B395" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="C395" t="s">
-        <v>1567</v>
+        <v>1564</v>
       </c>
       <c r="D395" t="s">
-        <v>1568</v>
+        <v>1565</v>
       </c>
       <c r="E395" t="s">
-        <v>1580</v>
+        <v>1576</v>
       </c>
       <c r="F395" s="1" t="s">
-        <v>1577</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="396" spans="1:6" x14ac:dyDescent="0.3">
@@ -13609,19 +13612,19 @@
         <v>396</v>
       </c>
       <c r="B396" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="C396" t="s">
-        <v>1569</v>
+        <v>1566</v>
       </c>
       <c r="D396" t="s">
-        <v>1570</v>
+        <v>1567</v>
       </c>
       <c r="E396" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="F396" s="1" t="s">
-        <v>1577</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="397" spans="1:6" x14ac:dyDescent="0.3">
@@ -13630,19 +13633,19 @@
         <v>397</v>
       </c>
       <c r="B397" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="C397" t="s">
-        <v>1571</v>
+        <v>1631</v>
       </c>
       <c r="D397" t="s">
-        <v>1572</v>
+        <v>1568</v>
       </c>
       <c r="E397" t="s">
-        <v>1585</v>
+        <v>1581</v>
       </c>
       <c r="F397" s="1" t="s">
-        <v>1577</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="398" spans="1:6" x14ac:dyDescent="0.3">
@@ -13651,19 +13654,19 @@
         <v>398</v>
       </c>
       <c r="B398" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="C398" t="s">
+        <v>1569</v>
+      </c>
+      <c r="D398" t="s">
+        <v>1570</v>
+      </c>
+      <c r="E398" t="s">
+        <v>1582</v>
+      </c>
+      <c r="F398" s="1" t="s">
         <v>1573</v>
-      </c>
-      <c r="D398" t="s">
-        <v>1574</v>
-      </c>
-      <c r="E398" t="s">
-        <v>1586</v>
-      </c>
-      <c r="F398" s="1" t="s">
-        <v>1577</v>
       </c>
     </row>
     <row r="399" spans="1:6" x14ac:dyDescent="0.3">
@@ -13672,19 +13675,19 @@
         <v>399</v>
       </c>
       <c r="B399" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="C399" t="s">
-        <v>1575</v>
+        <v>1571</v>
       </c>
       <c r="D399" t="s">
-        <v>1576</v>
+        <v>1572</v>
       </c>
       <c r="E399" t="s">
-        <v>1587</v>
+        <v>1583</v>
       </c>
       <c r="F399" s="1" t="s">
-        <v>1577</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="400" spans="1:6" x14ac:dyDescent="0.3">
@@ -13693,19 +13696,19 @@
         <v>400</v>
       </c>
       <c r="B400" t="s">
-        <v>1598</v>
+        <v>1594</v>
       </c>
       <c r="C400" t="s">
-        <v>1599</v>
+        <v>1595</v>
       </c>
       <c r="D400" t="s">
-        <v>1601</v>
+        <v>1596</v>
       </c>
       <c r="E400" t="s">
-        <v>1600</v>
+        <v>1633</v>
       </c>
       <c r="F400" s="1" t="s">
-        <v>1640</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="401" spans="1:6" x14ac:dyDescent="0.3">
@@ -13714,19 +13717,19 @@
         <v>401</v>
       </c>
       <c r="B401" t="s">
+        <v>1594</v>
+      </c>
+      <c r="C401" t="s">
+        <v>1597</v>
+      </c>
+      <c r="D401" t="s">
         <v>1598</v>
       </c>
-      <c r="C401" t="s">
-        <v>1602</v>
-      </c>
-      <c r="D401" t="s">
-        <v>1603</v>
-      </c>
       <c r="E401" t="s">
-        <v>1604</v>
+        <v>1634</v>
       </c>
       <c r="F401" s="1" t="s">
-        <v>1640</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="402" spans="1:6" x14ac:dyDescent="0.3">
@@ -13735,19 +13738,19 @@
         <v>402</v>
       </c>
       <c r="B402" t="s">
-        <v>1598</v>
+        <v>1594</v>
       </c>
       <c r="C402" t="s">
-        <v>1606</v>
+        <v>1600</v>
       </c>
       <c r="D402" t="s">
-        <v>1605</v>
+        <v>1599</v>
       </c>
       <c r="E402" t="s">
-        <v>1607</v>
+        <v>1636</v>
       </c>
       <c r="F402" s="1" t="s">
-        <v>1640</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="403" spans="1:6" x14ac:dyDescent="0.3">
@@ -13756,19 +13759,19 @@
         <v>403</v>
       </c>
       <c r="B403" t="s">
-        <v>1598</v>
+        <v>1594</v>
       </c>
       <c r="C403" t="s">
-        <v>1608</v>
+        <v>1601</v>
       </c>
       <c r="D403" t="s">
-        <v>1609</v>
+        <v>1602</v>
       </c>
       <c r="E403" t="s">
-        <v>1610</v>
+        <v>1637</v>
       </c>
       <c r="F403" s="1" t="s">
-        <v>1640</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="404" spans="1:6" x14ac:dyDescent="0.3">
@@ -13777,19 +13780,19 @@
         <v>404</v>
       </c>
       <c r="B404" t="s">
-        <v>1598</v>
+        <v>1594</v>
       </c>
       <c r="C404" t="s">
-        <v>1611</v>
+        <v>1603</v>
       </c>
       <c r="D404" t="s">
-        <v>1612</v>
+        <v>1604</v>
       </c>
       <c r="E404" t="s">
-        <v>1610</v>
+        <v>1637</v>
       </c>
       <c r="F404" s="1" t="s">
-        <v>1640</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="405" spans="1:6" x14ac:dyDescent="0.3">
@@ -13798,19 +13801,19 @@
         <v>405</v>
       </c>
       <c r="B405" t="s">
-        <v>1598</v>
+        <v>1594</v>
       </c>
       <c r="C405" t="s">
-        <v>1613</v>
+        <v>1605</v>
       </c>
       <c r="D405" t="s">
-        <v>1614</v>
+        <v>1606</v>
       </c>
       <c r="E405" t="s">
-        <v>1615</v>
+        <v>1638</v>
       </c>
       <c r="F405" s="1" t="s">
-        <v>1640</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="406" spans="1:6" x14ac:dyDescent="0.3">
@@ -13819,19 +13822,19 @@
         <v>406</v>
       </c>
       <c r="B406" t="s">
-        <v>1598</v>
+        <v>1594</v>
       </c>
       <c r="C406" t="s">
-        <v>1617</v>
+        <v>1608</v>
       </c>
       <c r="D406" t="s">
-        <v>1616</v>
+        <v>1607</v>
       </c>
       <c r="E406" t="s">
-        <v>1618</v>
+        <v>1639</v>
       </c>
       <c r="F406" s="1" t="s">
-        <v>1640</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="407" spans="1:6" x14ac:dyDescent="0.3">
@@ -13840,19 +13843,19 @@
         <v>407</v>
       </c>
       <c r="B407" t="s">
-        <v>1598</v>
+        <v>1594</v>
       </c>
       <c r="C407" t="s">
-        <v>1619</v>
+        <v>1609</v>
       </c>
       <c r="D407" s="3" t="s">
-        <v>1620</v>
+        <v>1610</v>
       </c>
       <c r="E407" t="s">
-        <v>1621</v>
+        <v>1611</v>
       </c>
       <c r="F407" s="1" t="s">
-        <v>1640</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="408" spans="1:6" x14ac:dyDescent="0.3">
@@ -13861,19 +13864,19 @@
         <v>408</v>
       </c>
       <c r="B408" t="s">
-        <v>1598</v>
+        <v>1594</v>
       </c>
       <c r="C408" t="s">
-        <v>1622</v>
+        <v>1612</v>
       </c>
       <c r="D408" s="3" t="s">
-        <v>1623</v>
+        <v>1613</v>
       </c>
       <c r="E408" t="s">
-        <v>1624</v>
+        <v>1614</v>
       </c>
       <c r="F408" s="1" t="s">
-        <v>1640</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="409" spans="1:6" x14ac:dyDescent="0.3">
@@ -13882,19 +13885,19 @@
         <v>409</v>
       </c>
       <c r="B409" t="s">
-        <v>1598</v>
+        <v>1594</v>
       </c>
       <c r="C409" t="s">
+        <v>1615</v>
+      </c>
+      <c r="D409" t="s">
+        <v>1616</v>
+      </c>
+      <c r="E409" t="s">
+        <v>1640</v>
+      </c>
+      <c r="F409" s="1" t="s">
         <v>1625</v>
-      </c>
-      <c r="D409" t="s">
-        <v>1626</v>
-      </c>
-      <c r="E409" t="s">
-        <v>1627</v>
-      </c>
-      <c r="F409" s="1" t="s">
-        <v>1640</v>
       </c>
     </row>
     <row r="410" spans="1:6" x14ac:dyDescent="0.3">
@@ -13903,19 +13906,19 @@
         <v>410</v>
       </c>
       <c r="B410" t="s">
-        <v>1598</v>
+        <v>1594</v>
       </c>
       <c r="C410" t="s">
-        <v>1629</v>
+        <v>1618</v>
       </c>
       <c r="D410" t="s">
-        <v>1628</v>
+        <v>1617</v>
       </c>
       <c r="E410" t="s">
-        <v>1630</v>
+        <v>1632</v>
       </c>
       <c r="F410" s="1" t="s">
-        <v>1640</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="411" spans="1:6" x14ac:dyDescent="0.3">
@@ -13924,19 +13927,19 @@
         <v>411</v>
       </c>
       <c r="B411" t="s">
-        <v>1598</v>
+        <v>1594</v>
       </c>
       <c r="C411" t="s">
-        <v>1631</v>
+        <v>1619</v>
       </c>
       <c r="D411" t="s">
-        <v>1632</v>
+        <v>1620</v>
       </c>
       <c r="E411" t="s">
-        <v>1633</v>
+        <v>1641</v>
       </c>
       <c r="F411" s="1" t="s">
-        <v>1640</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="412" spans="1:6" x14ac:dyDescent="0.3">
@@ -13945,19 +13948,19 @@
         <v>412</v>
       </c>
       <c r="B412" t="s">
-        <v>1598</v>
+        <v>1594</v>
       </c>
       <c r="C412" t="s">
-        <v>1634</v>
+        <v>1621</v>
       </c>
       <c r="D412" t="s">
-        <v>1635</v>
+        <v>1622</v>
       </c>
       <c r="E412" t="s">
-        <v>1636</v>
+        <v>1642</v>
       </c>
       <c r="F412" s="1" t="s">
-        <v>1640</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="413" spans="1:6" x14ac:dyDescent="0.3">
@@ -13966,19 +13969,19 @@
         <v>413</v>
       </c>
       <c r="B413" t="s">
-        <v>1598</v>
+        <v>1594</v>
       </c>
       <c r="C413" t="s">
-        <v>1637</v>
+        <v>1623</v>
       </c>
       <c r="D413" t="s">
-        <v>1638</v>
+        <v>1624</v>
       </c>
       <c r="E413" t="s">
-        <v>1639</v>
+        <v>1635</v>
       </c>
       <c r="F413" s="1" t="s">
-        <v>1640</v>
+        <v>1625</v>
       </c>
     </row>
   </sheetData>
@@ -14003,17 +14006,17 @@
     <hyperlink ref="F335" r:id="rId18"/>
     <hyperlink ref="F336:F368" r:id="rId19" display="file:///android_asset/shopping.png"/>
     <hyperlink ref="F370" r:id="rId20"/>
-    <hyperlink ref="F371:F379" r:id="rId21" display="file:///android_asset/getting_around.png"/>
-    <hyperlink ref="F2" r:id="rId22"/>
-    <hyperlink ref="F37" r:id="rId23"/>
-    <hyperlink ref="F380" r:id="rId24"/>
-    <hyperlink ref="F39" r:id="rId25"/>
-    <hyperlink ref="F40" r:id="rId26"/>
-    <hyperlink ref="F38" r:id="rId27"/>
-    <hyperlink ref="F369" r:id="rId28"/>
-    <hyperlink ref="F381:F399" r:id="rId29" display="file:///android_asset/love.png"/>
-    <hyperlink ref="F400" r:id="rId30"/>
-    <hyperlink ref="F401:F413" r:id="rId31" display="file:///android_asset/medical.png"/>
+    <hyperlink ref="F2" r:id="rId21"/>
+    <hyperlink ref="F37" r:id="rId22"/>
+    <hyperlink ref="F380" r:id="rId23"/>
+    <hyperlink ref="F39" r:id="rId24"/>
+    <hyperlink ref="F40" r:id="rId25"/>
+    <hyperlink ref="F38" r:id="rId26"/>
+    <hyperlink ref="F369" r:id="rId27"/>
+    <hyperlink ref="F381:F399" r:id="rId28" display="file:///android_asset/love.png"/>
+    <hyperlink ref="F400" r:id="rId29"/>
+    <hyperlink ref="F401:F413" r:id="rId30" display="file:///android_asset/medical.png"/>
+    <hyperlink ref="F371:F379" r:id="rId31" display="file:///android_asset/driving.png"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated google TTS check.  hide speaker button if now google tts available
</commit_message>
<xml_diff>
--- a/app/src/main/assets/Cantonese Phrases.xlsx
+++ b/app/src/main/assets/Cantonese Phrases.xlsx
@@ -5586,9 +5586,6 @@
     <t>你哋收唔收 加 元嘎?</t>
   </si>
   <si>
-    <t>Do you accept AmericanCanadian dollars?</t>
-  </si>
-  <si>
     <t>Do you accept Australian dollars?</t>
   </si>
   <si>
@@ -5695,6 +5692,9 @@
   </si>
   <si>
     <t xml:space="preserve">今日天氣 </t>
+  </si>
+  <si>
+    <t>Do you accept American dollars?</t>
   </si>
 </sst>
 </file>
@@ -6044,7 +6044,7 @@
   <dimension ref="A1:F495"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10600,13 +10600,13 @@
         <v>398</v>
       </c>
       <c r="C217" t="s">
-        <v>1853</v>
+        <v>1889</v>
       </c>
       <c r="D217" t="s">
         <v>1850</v>
       </c>
       <c r="E217" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
       <c r="F217" s="1" t="s">
         <v>434</v>
@@ -10621,13 +10621,13 @@
         <v>398</v>
       </c>
       <c r="C218" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="D218" t="s">
         <v>1851</v>
       </c>
       <c r="E218" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="F218" s="1" t="s">
         <v>434</v>
@@ -10642,13 +10642,13 @@
         <v>398</v>
       </c>
       <c r="C219" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="D219" t="s">
         <v>1852</v>
       </c>
       <c r="E219" t="s">
-        <v>1860</v>
+        <v>1859</v>
       </c>
       <c r="F219" s="1" t="s">
         <v>434</v>
@@ -10663,13 +10663,13 @@
         <v>398</v>
       </c>
       <c r="C220" t="s">
+        <v>1855</v>
+      </c>
+      <c r="D220" t="s">
         <v>1856</v>
       </c>
-      <c r="D220" t="s">
-        <v>1857</v>
-      </c>
       <c r="E220" t="s">
-        <v>1861</v>
+        <v>1860</v>
       </c>
       <c r="F220" s="1" t="s">
         <v>434</v>
@@ -13060,7 +13060,7 @@
         <v>729</v>
       </c>
       <c r="D334" t="s">
-        <v>1862</v>
+        <v>1861</v>
       </c>
       <c r="E334" t="s">
         <v>1003</v>
@@ -13081,7 +13081,7 @@
         <v>730</v>
       </c>
       <c r="D335" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="E335" t="s">
         <v>1004</v>
@@ -13102,7 +13102,7 @@
         <v>731</v>
       </c>
       <c r="D336" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="E336" t="s">
         <v>1005</v>
@@ -13123,7 +13123,7 @@
         <v>732</v>
       </c>
       <c r="D337" t="s">
-        <v>1865</v>
+        <v>1864</v>
       </c>
       <c r="E337" t="s">
         <v>1006</v>
@@ -13144,7 +13144,7 @@
         <v>733</v>
       </c>
       <c r="D338" t="s">
-        <v>1866</v>
+        <v>1865</v>
       </c>
       <c r="E338" t="s">
         <v>1007</v>
@@ -13165,7 +13165,7 @@
         <v>734</v>
       </c>
       <c r="D339" t="s">
-        <v>1867</v>
+        <v>1866</v>
       </c>
       <c r="E339" t="s">
         <v>1011</v>
@@ -13186,7 +13186,7 @@
         <v>735</v>
       </c>
       <c r="D340" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="E340" t="s">
         <v>1012</v>
@@ -13207,7 +13207,7 @@
         <v>736</v>
       </c>
       <c r="D341" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="E341" t="s">
         <v>1013</v>
@@ -13228,7 +13228,7 @@
         <v>737</v>
       </c>
       <c r="D342" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="E342" t="s">
         <v>1014</v>
@@ -13249,7 +13249,7 @@
         <v>738</v>
       </c>
       <c r="D343" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
       <c r="E343" t="s">
         <v>1015</v>
@@ -13270,7 +13270,7 @@
         <v>1827</v>
       </c>
       <c r="D344" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
       <c r="E344" t="s">
         <v>1683</v>
@@ -13291,7 +13291,7 @@
         <v>1684</v>
       </c>
       <c r="D345" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="E345" t="s">
         <v>1685</v>
@@ -13312,7 +13312,7 @@
         <v>1828</v>
       </c>
       <c r="D346" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="E346" t="s">
         <v>1686</v>
@@ -13333,7 +13333,7 @@
         <v>1689</v>
       </c>
       <c r="D347" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="E347" t="s">
         <v>1687</v>
@@ -13354,7 +13354,7 @@
         <v>1688</v>
       </c>
       <c r="D348" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="E348" t="s">
         <v>1690</v>
@@ -13375,7 +13375,7 @@
         <v>1691</v>
       </c>
       <c r="D349" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="E349" t="s">
         <v>1692</v>
@@ -13396,7 +13396,7 @@
         <v>1693</v>
       </c>
       <c r="D350" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
       <c r="E350" t="s">
         <v>1694</v>
@@ -13417,7 +13417,7 @@
         <v>1695</v>
       </c>
       <c r="D351" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
       <c r="E351" t="s">
         <v>1696</v>
@@ -13438,7 +13438,7 @@
         <v>1697</v>
       </c>
       <c r="D352" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="E352" t="s">
         <v>1698</v>
@@ -13459,7 +13459,7 @@
         <v>1699</v>
       </c>
       <c r="D353" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="E353" t="s">
         <v>1700</v>
@@ -13480,7 +13480,7 @@
         <v>1701</v>
       </c>
       <c r="D354" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="E354" t="s">
         <v>1702</v>
@@ -13984,7 +13984,7 @@
         <v>1612</v>
       </c>
       <c r="D378" t="s">
-        <v>1887</v>
+        <v>1886</v>
       </c>
       <c r="E378" t="s">
         <v>1613</v>
@@ -14509,7 +14509,7 @@
         <v>1582</v>
       </c>
       <c r="D403" t="s">
-        <v>1888</v>
+        <v>1887</v>
       </c>
       <c r="E403" t="s">
         <v>1776</v>
@@ -14971,7 +14971,7 @@
         <v>1631</v>
       </c>
       <c r="D425" t="s">
-        <v>1872</v>
+        <v>1871</v>
       </c>
       <c r="E425" t="s">
         <v>1008</v>
@@ -14992,7 +14992,7 @@
         <v>1632</v>
       </c>
       <c r="D426" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="E426" t="s">
         <v>1009</v>
@@ -15013,7 +15013,7 @@
         <v>1633</v>
       </c>
       <c r="D427" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="E427" t="s">
         <v>1010</v>
@@ -15097,7 +15097,7 @@
         <v>1480</v>
       </c>
       <c r="D431" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="E431" t="s">
         <v>1611</v>
@@ -15874,7 +15874,7 @@
         <v>1718</v>
       </c>
       <c r="D468" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="E468" s="5" t="s">
         <v>1717</v>

</xml_diff>